<commit_message>
ajout de x-decor à la liste (semble interressant mais à tester côté lag).
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="172">
   <si>
     <t>génération map</t>
   </si>
@@ -361,6 +361,18 @@
   </si>
   <si>
     <t>https://github.com/VanessaE/homedecor_modpack</t>
+  </si>
+  <si>
+    <t>X decor</t>
+  </si>
+  <si>
+    <t>comme homedecor mais en mieux</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=12534</t>
+  </si>
+  <si>
+    <t>https://github.com/kilbith/xdecor</t>
   </si>
   <si>
     <t>Génération/embellissement carte</t>
@@ -1503,10 +1515,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:E56"/>
+  <dimension ref="B1:E57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1519,6 +1531,14 @@
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
         <v>76</v>
@@ -1559,6 +1579,14 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
         <v>83</v>
@@ -1608,6 +1636,14 @@
       <c r="E12" s="6" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
@@ -1661,6 +1697,10 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
         <v>97</v>
@@ -1707,6 +1747,10 @@
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
     </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+    </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="s">
         <v>101</v>
@@ -1799,115 +1843,127 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0"/>
-      <c r="C34" s="0"/>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+    <row r="39" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="13" t="s">
-        <v>126</v>
-      </c>
       <c r="C46" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="13" t="s">
         <v>130</v>
       </c>
@@ -1921,7 +1977,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="13" t="s">
         <v>134</v>
       </c>
@@ -1931,23 +1987,23 @@
       <c r="D48" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" s="5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
         <v>141</v>
       </c>
@@ -1957,23 +2013,23 @@
       <c r="D50" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
         <v>148</v>
       </c>
@@ -1987,7 +2043,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
         <v>152</v>
       </c>
@@ -2001,7 +2057,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
         <v>156</v>
       </c>
@@ -2015,7 +2071,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
         <v>160</v>
       </c>
@@ -2029,7 +2085,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
         <v>164</v>
       </c>
@@ -2041,6 +2097,20 @@
       </c>
       <c r="E56" s="5" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2050,8 +2120,8 @@
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B43:E43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
nouvelle mise à jour de la liste.
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="144" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="173" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propositions joueurs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="175">
   <si>
     <t>génération map</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Survie</t>
   </si>
   <si>
-    <t>bones</t>
-  </si>
-  <si>
-    <t>Place le contenu de l'inventaire du joueur dans un bloc à sa mort</t>
-  </si>
-  <si>
     <t>hud</t>
   </si>
   <si>
@@ -309,16 +303,31 @@
     <t>https://github.com/BlockMen/hunger</t>
   </si>
   <si>
+    <t>farming_plus</t>
+  </si>
+  <si>
+    <t>supplément d'item à farming</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=2787</t>
+  </si>
+  <si>
+    <t>https://github.com/PilzAdam/farming_plus</t>
+  </si>
+  <si>
     <t>Animaux/Pnj</t>
   </si>
   <si>
-    <t>kpgmods</t>
+    <t>mob redo</t>
   </si>
   <si>
     <t>Ajoute plein d'animaux différents</t>
   </si>
   <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=8798&amp;sid=b534e2f159bba6c0641601986cd4de9d</t>
+    <t>https://forum.minetest.net/viewtopic.php?t=9917</t>
+  </si>
+  <si>
+    <t>https://github.com/tenplus1/mobs</t>
   </si>
   <si>
     <t>Construction</t>
@@ -378,18 +387,6 @@
     <t>Génération/embellissement carte</t>
   </si>
   <si>
-    <t>mg : experimental mapgen</t>
-  </si>
-  <si>
-    <t>génération de montagnes, cave, villages…</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=7263&amp;sid=812e62edc02830d766bf465926ce8913</t>
-  </si>
-  <si>
-    <t>https://github.com/Novatux/mg</t>
-  </si>
-  <si>
     <t>worldedit</t>
   </si>
   <si>
@@ -532,6 +529,18 @@
   </si>
   <si>
     <t>https://github.com/bas080/inbox</t>
+  </si>
+  <si>
+    <t>bags</t>
+  </si>
+  <si>
+    <t>sacs pour stocker des items</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=3081</t>
+  </si>
+  <si>
+    <t>https://github.com/cornernote/minetest-bags</t>
   </si>
 </sst>
 </file>
@@ -1515,15 +1524,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E57"/>
+  <dimension ref="B1:E58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.27551020408163"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="9" width="22.1734693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="26.6836734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.0510204081633"/>
@@ -1667,28 +1676,32 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1716,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1723,17 +1736,19 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13"/>
@@ -1753,7 +1768,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1773,29 +1788,29 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>29</v>
@@ -1806,10 +1821,10 @@
         <v>14</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>16</v>
@@ -1817,44 +1832,44 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="13" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,7 +1882,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1887,19 +1902,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>123</v>
-      </c>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="13"/>
@@ -1937,180 +1944,194 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="D45" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="13" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="E46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="D47" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E47" s="5" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="13" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="D48" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="D49" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="D50" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E50" s="5" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="13" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="D51" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="D52" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E52" s="5" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="13" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="D53" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E53" s="5" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="13" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="13" t="s">
+      <c r="C54" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="D54" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="5" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="13" t="s">
+      <c r="C55" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="D55" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="D56" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="E56" s="5" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="13" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="13" t="s">
+      <c r="C57" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="D57" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E57" s="5" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="13" t="s">
         <v>171</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Première version du gamemod (pas de sous module)
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="173" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propositions joueurs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="200">
   <si>
     <t>génération map</t>
   </si>
@@ -288,259 +288,334 @@
     <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=11437&amp;sid=812e62edc02830d766bf465926ce8913</t>
   </si>
   <si>
+    <t>https://gitlab.com/echoes91/throwing.git</t>
+  </si>
+  <si>
     <t>Survie</t>
   </si>
   <si>
+    <t>hunger</t>
+  </si>
+  <si>
+    <t>Ajoute la faim dans le jeu</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=6342</t>
+  </si>
+  <si>
+    <t>https://github.com/BlockMen/hunger</t>
+  </si>
+  <si>
+    <t>farming_plus</t>
+  </si>
+  <si>
+    <t>supplément d'item à farming</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=2787</t>
+  </si>
+  <si>
+    <t>https://github.com/PilzAdam/farming_plus</t>
+  </si>
+  <si>
+    <t>le joueur prend des coup s'il se retrouve sous du sable ou des graviers</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=2638</t>
+  </si>
+  <si>
+    <t>Animaux/Pnj</t>
+  </si>
+  <si>
+    <t>mob redo</t>
+  </si>
+  <si>
+    <t>Ajoute plein d'animaux différents</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?t=9917</t>
+  </si>
+  <si>
+    <t>https://github.com/tenplus1/mobs</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Transport d'items et craft automatisé</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=2155</t>
+  </si>
+  <si>
+    <t>Circuits électrique et automatisation</t>
+  </si>
+  <si>
+    <t>http://mesecons.net/</t>
+  </si>
+  <si>
+    <t>Supplément de blocs</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=509</t>
+  </si>
+  <si>
+    <t>coloured stone brick</t>
+  </si>
+  <si>
+    <t>Des blocs coloré et éditable avec la scie circulaire</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=8784</t>
+  </si>
+  <si>
+    <t>https://github.com/CraigyDavi/colouredstonebricks</t>
+  </si>
+  <si>
+    <t>Plein d'items et de blocks pour la décoration</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=2041</t>
+  </si>
+  <si>
+    <t>https://github.com/VanessaE/homedecor_modpack</t>
+  </si>
+  <si>
+    <t>X decor</t>
+  </si>
+  <si>
+    <t>comme homedecor mais en mieux</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=12534</t>
+  </si>
+  <si>
+    <t>https://github.com/kilbith/xdecor</t>
+  </si>
+  <si>
+    <t>arrow sign</t>
+  </si>
+  <si>
+    <t>des panneaux avec une fleche</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?pid=99655</t>
+  </si>
+  <si>
+    <t>Génération/embellissement carte</t>
+  </si>
+  <si>
+    <t>default plus</t>
+  </si>
+  <si>
+    <t>ajoute quelques améliorations aux textures et au gameplay</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=6033&amp;hilit=dplus&amp;sid=a2d0c40dbb5fd3c4bcb0dac2b5da0b30</t>
+  </si>
+  <si>
+    <t>worldedit</t>
+  </si>
+  <si>
+    <t>opérations spécifiques directement sur la carte</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=572</t>
+  </si>
+  <si>
+    <t>https://github.com/Uberi/Minetest-WorldEdit</t>
+  </si>
+  <si>
+    <t>Oblige le nouveau joueur à accepter les règles du serveur</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=12441</t>
+  </si>
+  <si>
+    <t>connected_chest</t>
+  </si>
+  <si>
+    <t>Création de coffre double</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=10264</t>
+  </si>
+  <si>
+    <t>https://github.com/HybridDog/connected_chests</t>
+  </si>
+  <si>
+    <t>locked shared chest</t>
+  </si>
+  <si>
+    <t>permet aux joueurs de partager le contenu de leur coffres</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=3653</t>
+  </si>
+  <si>
+    <t>https://github.com/Sokomine/locks</t>
+  </si>
+  <si>
+    <t>helicopter</t>
+  </si>
+  <si>
+    <t>un helicopter fonctionnel</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=6183</t>
+  </si>
+  <si>
+    <t>cubic microcar</t>
+  </si>
+  <si>
+    <t>De petites voitures fonctionnelles</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?t=7967</t>
+  </si>
+  <si>
+    <t>https://github.com/paramat/mesecar</t>
+  </si>
+  <si>
+    <t>monorail</t>
+  </si>
+  <si>
+    <t>wagons capable de transporter des chest</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?t=730</t>
+  </si>
+  <si>
+    <t>beds</t>
+  </si>
+  <si>
+    <t>des lits pour respawner</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9881&amp;hilit=player+texture&amp;sid=03eecdb7fb85ba244804a47caaa23cf0</t>
+  </si>
+  <si>
+    <t>https://github.com/BlockMen/beds</t>
+  </si>
+  <si>
+    <t>in game skin switching</t>
+  </si>
+  <si>
+    <t>Textures personnalisée pour les joueurs, changeable dans le jeu</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=4147&amp;hilit=texture&amp;sid=03eecdb7fb85ba244804a47caaa23cf0</t>
+  </si>
+  <si>
+    <t>https://github.com/Zeg9/minetest-skins</t>
+  </si>
+  <si>
+    <t>markers</t>
+  </si>
+  <si>
+    <t>Permet au joueurs de protéger leur construction d'une manière graphique</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=8175</t>
+  </si>
+  <si>
+    <t>https://github.com/Sokomine/markers</t>
+  </si>
+  <si>
+    <t>areas</t>
+  </si>
+  <si>
+    <t>dépendance obligatoire pour markers</t>
+  </si>
+  <si>
+    <t>https://github.com/ShadowNinja/areas</t>
+  </si>
+  <si>
+    <t>inventory++</t>
+  </si>
+  <si>
+    <t>items supplémentaires pour les menus</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=6204</t>
+  </si>
+  <si>
+    <t>https://github.com/Zeg9/minetest-inventory_plus</t>
+  </si>
+  <si>
+    <t>memorandum</t>
+  </si>
+  <si>
+    <t>Permet d'écrire sur les papiers</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=6945&amp;sid=79d9cdf15fe565bf09071b6a3e34a7ce</t>
+  </si>
+  <si>
+    <t>https://github.com/Mossmanikin/memorandum</t>
+  </si>
+  <si>
+    <t>inbox</t>
+  </si>
+  <si>
+    <t>permet d'échanger des messages et des items entre joueurs</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?pid=107656#p107656</t>
+  </si>
+  <si>
+    <t>https://github.com/bas080/inbox</t>
+  </si>
+  <si>
+    <t>bags</t>
+  </si>
+  <si>
+    <t>sacs pour stocker des items</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=3081</t>
+  </si>
+  <si>
+    <t>https://github.com/cornernote/minetest-bags</t>
+  </si>
+  <si>
+    <t>zcg</t>
+  </si>
+  <si>
+    <t>craft guide dans l'inventaire du joueur</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=5564&amp;sid=7a0238a8581564907410b721dbd079d3</t>
+  </si>
+  <si>
+    <t>https://github.com/Zeg9/minetest-zcg</t>
+  </si>
+  <si>
     <t>hud</t>
   </si>
   <si>
-    <t>Ajoute la faim dans le jeu</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=6342</t>
-  </si>
-  <si>
-    <t>https://github.com/BlockMen/hunger</t>
-  </si>
-  <si>
-    <t>farming_plus</t>
-  </si>
-  <si>
-    <t>supplément d'item à farming</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=2787</t>
-  </si>
-  <si>
-    <t>https://github.com/PilzAdam/farming_plus</t>
-  </si>
-  <si>
-    <t>Animaux/Pnj</t>
-  </si>
-  <si>
-    <t>mob redo</t>
-  </si>
-  <si>
-    <t>Ajoute plein d'animaux différents</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?t=9917</t>
-  </si>
-  <si>
-    <t>https://github.com/tenplus1/mobs</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Transport d'items et craft automatisé</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=2155</t>
-  </si>
-  <si>
-    <t>Circuits électrique et automatisation</t>
-  </si>
-  <si>
-    <t>http://mesecons.net/</t>
-  </si>
-  <si>
-    <t>Supplément de blocs</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=509</t>
-  </si>
-  <si>
-    <t>coloured stone brick</t>
-  </si>
-  <si>
-    <t>Des blocs coloré et éditable avec la scie circulaire</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=8784</t>
-  </si>
-  <si>
-    <t>https://github.com/CraigyDavi/colouredstonebricks</t>
-  </si>
-  <si>
-    <t>Plein d'items et de blocks pour la décoration</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=2041</t>
-  </si>
-  <si>
-    <t>https://github.com/VanessaE/homedecor_modpack</t>
-  </si>
-  <si>
-    <t>X decor</t>
-  </si>
-  <si>
-    <t>comme homedecor mais en mieux</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=12534</t>
-  </si>
-  <si>
-    <t>https://github.com/kilbith/xdecor</t>
-  </si>
-  <si>
-    <t>Génération/embellissement carte</t>
-  </si>
-  <si>
-    <t>worldedit</t>
-  </si>
-  <si>
-    <t>opérations spécifiques directement sur la carte</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=572</t>
-  </si>
-  <si>
-    <t>https://github.com/Uberi/Minetest-WorldEdit</t>
-  </si>
-  <si>
-    <t>Oblige le nouveau joueur à accepter les règles du serveur</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=12441</t>
-  </si>
-  <si>
-    <t>connected_chest</t>
-  </si>
-  <si>
-    <t>Création de coffre double</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=10264</t>
-  </si>
-  <si>
-    <t>https://github.com/HybridDog/connected_chests</t>
-  </si>
-  <si>
-    <t>locked shared chest</t>
-  </si>
-  <si>
-    <t>permet aux joueurs de partager le contenu de leur coffres</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=3653</t>
-  </si>
-  <si>
-    <t>https://github.com/Sokomine/locks</t>
-  </si>
-  <si>
-    <t>helicopter</t>
-  </si>
-  <si>
-    <t>un helicopter fonctionnel</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=6183</t>
-  </si>
-  <si>
-    <t>cubic microcar</t>
-  </si>
-  <si>
-    <t>De petites voitures fonctionnelles</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?t=7967</t>
-  </si>
-  <si>
-    <t>https://github.com/paramat/mesecar</t>
-  </si>
-  <si>
-    <t>monorail</t>
-  </si>
-  <si>
-    <t>wagons capable de transporter des chest</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?t=730</t>
-  </si>
-  <si>
-    <t>beds</t>
-  </si>
-  <si>
-    <t>des lits pour respawner</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9881&amp;hilit=player+texture&amp;sid=03eecdb7fb85ba244804a47caaa23cf0</t>
-  </si>
-  <si>
-    <t>https://github.com/BlockMen/beds</t>
-  </si>
-  <si>
-    <t>in game skin switching</t>
-  </si>
-  <si>
-    <t>Textures personnalisée pour les joueurs, changeable dans le jeu</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=4147&amp;hilit=texture&amp;sid=03eecdb7fb85ba244804a47caaa23cf0</t>
-  </si>
-  <si>
-    <t>https://github.com/Zeg9/minetest-skins</t>
-  </si>
-  <si>
-    <t>markers</t>
-  </si>
-  <si>
-    <t>Permet au joueurs de protéger leur construction d'une manière graphique</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=8175</t>
-  </si>
-  <si>
-    <t>https://github.com/Sokomine/markers</t>
-  </si>
-  <si>
-    <t>inventory++</t>
-  </si>
-  <si>
-    <t>items supplémentaires pour les menus</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=6204</t>
-  </si>
-  <si>
-    <t>https://github.com/Zeg9/minetest-inventory_plus</t>
-  </si>
-  <si>
-    <t>memorandum</t>
-  </si>
-  <si>
-    <t>Permet d'écrire sur les papiers</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=6945&amp;sid=79d9cdf15fe565bf09071b6a3e34a7ce</t>
-  </si>
-  <si>
-    <t>https://github.com/Mossmanikin/memorandum</t>
-  </si>
-  <si>
-    <t>inbox</t>
-  </si>
-  <si>
-    <t>permet d'échanger des messages et des items entre joueurs</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?pid=107656#p107656</t>
-  </si>
-  <si>
-    <t>https://github.com/bas080/inbox</t>
-  </si>
-  <si>
-    <t>bags</t>
-  </si>
-  <si>
-    <t>sacs pour stocker des items</t>
-  </si>
-  <si>
-    <t>https://forum.minetest.net/viewtopic.php?id=3081</t>
-  </si>
-  <si>
-    <t>https://github.com/cornernote/minetest-bags</t>
+    <t>ajoute la barre de faim dans la vue du joueur</t>
+  </si>
+  <si>
+    <t>https://github.com/BlockMen/hud</t>
+  </si>
+  <si>
+    <t>antiguest</t>
+  </si>
+  <si>
+    <t>empeche les joueurs qui ne prennent pas le temps de trouver un pseudo</t>
+  </si>
+  <si>
+    <t>buildin_item</t>
+  </si>
+  <si>
+    <t>les nodes et items sont poussé par l'eau et détruit dans la lave</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=3188</t>
+  </si>
+  <si>
+    <t>https://github.com/PilzAdam/builtin_item</t>
   </si>
 </sst>
 </file>
@@ -550,7 +625,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -585,8 +660,15 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,8 +683,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFAECF00"/>
-        <bgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFCCFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -660,7 +748,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -721,6 +809,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -733,12 +829,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -757,7 +877,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFCCFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -820,8 +940,8 @@
   </sheetPr>
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1524,10 +1644,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:E58"/>
+  <dimension ref="B1:F65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D65" activeCellId="0" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1535,18 +1655,21 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.27551020408163"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="9" width="22.1734693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="26.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="2.81632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="78.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="11" t="s">
@@ -1555,6 +1678,7 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
@@ -1563,38 +1687,43 @@
       <c r="C4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="11" t="s">
@@ -1603,6 +1732,7 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
@@ -1611,10 +1741,11 @@
       <c r="C10" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1625,10 +1756,11 @@
       <c r="C11" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1639,28 +1771,32 @@
       <c r="C12" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>61</v>
+      <c r="F12" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0"/>
       <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0"/>
       <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
@@ -1669,481 +1805,626 @@
       <c r="C16" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="12"/>
+      <c r="E16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="5" t="s">
         <v>93</v>
       </c>
+      <c r="D17" s="15"/>
       <c r="E17" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="F17" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="D18" s="15"/>
       <c r="E18" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="F18" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="5" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C29" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="12"/>
+      <c r="E29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13" t="s">
+    <row r="30" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="C30" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13" t="s">
+    <row r="31" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="C31" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="s">
-        <v>111</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="15"/>
+      <c r="E32" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>114</v>
+      <c r="F32" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="13" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="15"/>
+      <c r="E33" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="D34" s="15"/>
+      <c r="E34" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="5" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="13" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
+      <c r="C35" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="15"/>
+      <c r="E35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
+      <c r="B36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D40" s="12"/>
+      <c r="E40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
+    <row r="41" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4" t="s">
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C46" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D46" s="12"/>
+      <c r="E46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="13" t="s">
+    <row r="47" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="C48" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>135</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D48" s="15"/>
       <c r="E48" s="5" t="s">
-        <v>136</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="15"/>
+      <c r="E49" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>142</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D50" s="15"/>
       <c r="E50" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="5"/>
+        <v>147</v>
+      </c>
+      <c r="D51" s="15"/>
+      <c r="E51" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>149</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D52" s="15"/>
       <c r="E52" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>151</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>153</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D53" s="15"/>
       <c r="E53" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D54" s="5" t="s">
         <v>157</v>
       </c>
+      <c r="D54" s="15"/>
       <c r="E54" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" s="5" t="s">
         <v>161</v>
       </c>
+      <c r="D55" s="15"/>
       <c r="E55" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="5" t="s">
         <v>165</v>
       </c>
+      <c r="D56" s="15"/>
       <c r="E56" s="5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D57" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13" t="s">
         <v>171</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="15"/>
+      <c r="E58" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="F58" s="5" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D62" s="24"/>
+      <c r="E62" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="24"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+    </row>
+    <row r="65" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="D65" s="24"/>
+      <c r="E65" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B45:F45"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F12" r:id="rId1" display="https://gitlab.com/echoes91/throwing.git"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Ajout de bobblocks Ajout de watershed (génération de belles maps). Mise à jour du document tableur Mise à jour du .zip
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="166" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propositions joueurs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="209">
   <si>
     <t>génération map</t>
   </si>
@@ -402,6 +402,21 @@
     <t>https://forum.minetest.net/viewtopic.php?pid=99655</t>
   </si>
   <si>
+    <t>bobblocks</t>
+  </si>
+  <si>
+    <t>des blocs supplémentaires compatibles avec mesecons</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=1274</t>
+  </si>
+  <si>
+    <t>https://github.com/rabbibob/BobBlocks</t>
+  </si>
+  <si>
+    <t>attention a bien enlever les majuscules lors du clone du dépôt git</t>
+  </si>
+  <si>
     <t>Génération/embellissement carte</t>
   </si>
   <si>
@@ -412,6 +427,18 @@
   </si>
   <si>
     <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=6033&amp;hilit=dplus&amp;sid=a2d0c40dbb5fd3c4bcb0dac2b5da0b30</t>
+  </si>
+  <si>
+    <t>watershed</t>
+  </si>
+  <si>
+    <t>génére de belle map</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=8609&amp;sid=86bfda6d78747176347f2b459cc3e96e</t>
+  </si>
+  <si>
+    <t>https://github.com/paramat/watershed</t>
   </si>
   <si>
     <t>worldedit</t>
@@ -625,7 +652,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -667,8 +694,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,6 +718,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -829,14 +869,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -847,18 +899,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1644,10 +1684,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F65"/>
+  <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D65" activeCellId="0" sqref="D65"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2053,10 +2093,23 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
-      <c r="D37" s="0"/>
+    <row r="37" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0"/>
@@ -2064,53 +2117,61 @@
       <c r="D38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="3" t="s">
+      <c r="D41" s="12"/>
+      <c r="E41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="5"/>
+    <row r="42" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0"/>
-      <c r="C43" s="0"/>
-      <c r="D43" s="0"/>
+      <c r="B43" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="22"/>
+      <c r="E43" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0"/>
@@ -2118,298 +2179,303 @@
       <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C47" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="3" t="s">
+      <c r="D47" s="12"/>
+      <c r="E47" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="13" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>143</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="13" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>153</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="13" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23" t="s">
-        <v>170</v>
+        <v>174</v>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="13" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="13" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D61" s="24"/>
+        <v>189</v>
+      </c>
+      <c r="D61" s="15"/>
       <c r="E61" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="13" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="D62" s="24"/>
+        <v>193</v>
+      </c>
+      <c r="D62" s="27"/>
       <c r="E62" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="D63" s="24"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+      <c r="D63" s="27"/>
+      <c r="E63" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="13" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-    </row>
-    <row r="65" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="C65" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="F65" s="27" t="s">
-        <v>199</v>
+        <v>201</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D65" s="27"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+    </row>
+    <row r="66" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="27"/>
+      <c r="E66" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2419,11 +2485,12 @@
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B46:F46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1" display="https://gitlab.com/echoes91/throwing.git"/>
+    <hyperlink ref="F43" r:id="rId2" display="https://github.com/paramat/watershed"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Suppression de watershed Suppression de Nether Ajout de potions (pep) + dépendances nécessaire. MaJ du tableau de suivi MaJ du .zip pour les testeurs.
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="166" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="191" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propositions joueurs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="224">
   <si>
     <t>génération map</t>
   </si>
@@ -267,6 +267,48 @@
     <t>https://forum.minetest.net/viewtopic.php?id=7063</t>
   </si>
   <si>
+    <t>Accéder au monde du nether !</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=5790&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>https://github.com/PilzAdam/nether</t>
+  </si>
+  <si>
+    <t>on arrive contre un mur. Problème de génération du nether…</t>
+  </si>
+  <si>
+    <t>Potions</t>
+  </si>
+  <si>
+    <t>des potions magiques simple à crafter</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=10222&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>git://repo.or.cz/minetest_pep.git</t>
+  </si>
+  <si>
+    <t>!!! bien renommer le dépôt au moment du clonage</t>
+  </si>
+  <si>
+    <t>player effect</t>
+  </si>
+  <si>
+    <t>dépendance obligatoire pour potion</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9689</t>
+  </si>
+  <si>
+    <t>git://repo.or.cz/minetest_playereffects.git</t>
+  </si>
+  <si>
+    <t>!!! depends.txt vide, il faut ajouter « default » avant de lançer le jeu</t>
+  </si>
+  <si>
     <t>Action/combat</t>
   </si>
   <si>
@@ -439,6 +481,9 @@
   </si>
   <si>
     <t>https://github.com/paramat/watershed</t>
+  </si>
+  <si>
+    <t>inhibe les mod farming_plus et mobs redo. À enlever</t>
   </si>
   <si>
     <t>worldedit</t>
@@ -696,13 +741,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF800000"/>
+      <color rgb="FFFF6600"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,6 +764,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -788,7 +839,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -853,6 +904,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -869,15 +928,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -885,7 +944,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,7 +973,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFCCFF00"/>
@@ -981,7 +1040,7 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+      <selection pane="topLeft" activeCell="O10" activeCellId="1" sqref="9:9 O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1684,10 +1743,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G66"/>
+  <dimension ref="B1:G68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1698,7 +1757,8 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="2.81632653061224"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="78.0510204081633"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.5867346938775"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,748 +1809,800 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
+      <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="3" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="13" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
+      <c r="C13" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
+      <c r="B14" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C18" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="3" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="13" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
+      <c r="B20" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="3" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="B26" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="3" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13" t="s">
+    <row r="32" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="C32" s="14" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="13" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="5" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="5" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="13" t="s">
-        <v>125</v>
+        <v>48</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>133</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="13" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="20"/>
+        <v>136</v>
+      </c>
+      <c r="D37" s="15"/>
       <c r="E37" s="5" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
+      <c r="B38" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="3" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D42" s="15"/>
-      <c r="E42" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
+    <row r="44" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
+      <c r="B45" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="4" t="s">
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C49" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="3" t="s">
+      <c r="D49" s="12"/>
+      <c r="E49" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="5" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>164</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="5" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="5" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="5" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>179</v>
+      </c>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="13" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="5" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D58" s="25"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="5" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="13" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>193</v>
+      </c>
+      <c r="D60" s="27"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="13" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="5" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="13" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D62" s="27"/>
+        <v>200</v>
+      </c>
+      <c r="D62" s="15"/>
       <c r="E62" s="5" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D63" s="27"/>
+        <v>204</v>
+      </c>
+      <c r="D63" s="15"/>
       <c r="E63" s="5" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="13" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="26" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+      <c r="D64" s="29"/>
+      <c r="E64" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="13" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
+        <v>212</v>
+      </c>
+      <c r="D65" s="29"/>
+      <c r="E65" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="13" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+      <c r="D66" s="29"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D67" s="29"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+    </row>
+    <row r="68" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="D68" s="29"/>
+      <c r="E68" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B48:F48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1" display="https://gitlab.com/echoes91/throwing.git"/>
-    <hyperlink ref="F43" r:id="rId2" display="https://github.com/paramat/watershed"/>
+    <hyperlink ref="F14" r:id="rId1" display="https://gitlab.com/echoes91/throwing.git"/>
+    <hyperlink ref="F45" r:id="rId2" display="https://github.com/paramat/watershed"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Suppression de marker et area Ajout de : protector_redo, soccer, sprint, hoppers, my_corner. Mise à jour de .xlsx et du .zip
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="191" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="159" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propositions joueurs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="248">
   <si>
     <t>génération map</t>
   </si>
@@ -459,6 +459,18 @@
     <t>attention a bien enlever les majuscules lors du clone du dépôt git</t>
   </si>
   <si>
+    <t>my corner</t>
+  </si>
+  <si>
+    <t>intégration de coins coloré dans les blocks</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=11363&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>https://github.com/DonBatman/mycorners</t>
+  </si>
+  <si>
     <t>Génération/embellissement carte</t>
   </si>
   <si>
@@ -594,6 +606,9 @@
     <t>https://github.com/Sokomine/markers</t>
   </si>
   <si>
+    <t>pas pratique à utiliser</t>
+  </si>
+  <si>
     <t>areas</t>
   </si>
   <si>
@@ -688,6 +703,63 @@
   </si>
   <si>
     <t>https://github.com/PilzAdam/builtin_item</t>
+  </si>
+  <si>
+    <t>hoppers</t>
+  </si>
+  <si>
+    <t>les aspirateurs de mc !</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=12379&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>https://github.com/jordan4ibanez/Hoppers</t>
+  </si>
+  <si>
+    <t>!!!renommé le dossier « hopper » pour le clonage !!!</t>
+  </si>
+  <si>
+    <t>soccer</t>
+  </si>
+  <si>
+    <t>jouer à la baballe sur MT</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9662</t>
+  </si>
+  <si>
+    <t>https://github.com/kaeza/minetest-soccer</t>
+  </si>
+  <si>
+    <t>sprint</t>
+  </si>
+  <si>
+    <t>autorise le joueur à sprinter ponctuellement</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9650&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>https://github.com/GunshipPenguin/sprint</t>
+  </si>
+  <si>
+    <t>protection redo</t>
+  </si>
+  <si>
+    <t>blocs de protection de zone, panneaux, porte et chest protégés</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=11&amp;t=9376&amp;sid=80c275a032c5fa2972a28d1074f6f185</t>
+  </si>
+  <si>
+    <t>https://github.com/tenplus1/protector</t>
+  </si>
+  <si>
+    <t>suppression area et marker</t>
+  </si>
+  <si>
+    <t>ajout protection redo soccer sprint hoppers mycorner</t>
   </si>
 </sst>
 </file>
@@ -697,7 +769,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -733,6 +805,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -740,14 +819,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <strike val="true"/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,6 +878,12 @@
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
@@ -839,7 +933,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -904,15 +998,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -936,11 +1042,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -948,15 +1054,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="1" sqref="9:9 O10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1743,10 +1853,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G68"/>
+  <dimension ref="B1:G78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E79" activeCellId="0" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1808,18 +1918,18 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13" t="s">
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="19" t="s">
         <v>85</v>
       </c>
       <c r="G6" s="0" t="s">
@@ -1866,8 +1976,8 @@
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
       <c r="D9" s="0"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0"/>
@@ -1924,7 +2034,7 @@
       <c r="E14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="21" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2006,11 +2116,11 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0"/>
@@ -2064,11 +2174,11 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0"/>
@@ -2209,7 +2319,7 @@
       <c r="C39" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="22"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="5" t="s">
         <v>144</v>
       </c>
@@ -2220,10 +2330,20 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
+    <row r="40" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0"/>
@@ -2231,64 +2351,64 @@
       <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="3" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" s="24"/>
+        <v>153</v>
+      </c>
+      <c r="D45" s="15"/>
       <c r="E45" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F45" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="C46" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="27"/>
+      <c r="E46" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0"/>
@@ -2296,73 +2416,63 @@
       <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C50" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="3" t="s">
+      <c r="D50" s="12"/>
+      <c r="E50" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="13" t="s">
-        <v>62</v>
+        <v>160</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="13" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="13" t="s">
         <v>166</v>
       </c>
@@ -2377,7 +2487,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
         <v>170</v>
       </c>
@@ -2388,24 +2498,24 @@
       <c r="E54" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F55" s="5" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="13" t="s">
         <v>177</v>
       </c>
@@ -2416,24 +2526,24 @@
       <c r="E56" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F57" s="5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13" t="s">
         <v>184</v>
       </c>
@@ -2448,7 +2558,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13" t="s">
         <v>188</v>
       </c>
@@ -2463,131 +2573,225 @@
         <v>191</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="13" t="s">
+    <row r="60" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="D60" s="27"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28" t="s">
+      <c r="D60" s="18"/>
+      <c r="E60" s="19" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="13" t="s">
+      <c r="F60" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="G60" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="5" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="C61" s="17" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="30"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D64" s="29"/>
+        <v>209</v>
+      </c>
+      <c r="D64" s="15"/>
       <c r="E64" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="D65" s="29"/>
+        <v>213</v>
+      </c>
+      <c r="D65" s="31"/>
       <c r="E65" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D66" s="31"/>
+      <c r="E66" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="13" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-    </row>
-    <row r="68" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>221</v>
+      </c>
+      <c r="D67" s="31"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="13" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="D68" s="29"/>
-      <c r="E68" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="D68" s="31"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+    </row>
+    <row r="69" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" s="31"/>
+      <c r="E69" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D70" s="33"/>
+      <c r="E70" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D71" s="31"/>
+      <c r="E71" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D72" s="31"/>
+      <c r="E72" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D73" s="31"/>
+      <c r="E73" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2597,12 +2801,12 @@
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B49:F49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1" display="https://gitlab.com/echoes91/throwing.git"/>
-    <hyperlink ref="F45" r:id="rId2" display="https://github.com/paramat/watershed"/>
+    <hyperlink ref="F46" r:id="rId2" display="https://github.com/paramat/watershed"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ajout du mod firearms.
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="159" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mods du gamemods" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="194">
   <si>
     <t>Aventure</t>
   </si>
@@ -116,6 +116,21 @@
     <t>https://gitlab.com/echoes91/throwing.git</t>
   </si>
   <si>
+    <t>firearms</t>
+  </si>
+  <si>
+    <t>Armes à feu pour minetest</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?id=4562</t>
+  </si>
+  <si>
+    <t>https://github.com/kaeza/mt-firearms.git</t>
+  </si>
+  <si>
+    <t>Renommer le dossier en « firearms » au moment du clonage. Les armes à feu ne tuent pas les mobs de mob-redo !</t>
+  </si>
+  <si>
     <t>Survie</t>
   </si>
   <si>
@@ -567,6 +582,21 @@
   </si>
   <si>
     <t>https://github.com/tenplus1/protector</t>
+  </si>
+  <si>
+    <t>Enchantment</t>
+  </si>
+  <si>
+    <t>Enchantement permettant d'améliorer les outils</t>
+  </si>
+  <si>
+    <t>https://forum.minetest.net/viewtopic.php?f=9&amp;t=12641</t>
+  </si>
+  <si>
+    <t>https://github.com/jordan4ibanez/enchantment.git</t>
+  </si>
+  <si>
+    <t>ne fonctionne pas </t>
   </si>
 </sst>
 </file>
@@ -809,6 +839,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,10 +853,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -930,10 +960,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G72"/>
+  <dimension ref="B1:G74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E78" activeCellId="0" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -952,11 +982,13 @@
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
@@ -1065,6 +1097,7 @@
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
       <c r="D10" s="0"/>
+      <c r="G10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
@@ -1126,810 +1159,856 @@
       </c>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0"/>
       <c r="C16" s="0"/>
       <c r="D16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+      <c r="G16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="G17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+    <row r="22" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="G24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+    <row r="27" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="4" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="G29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6" t="s">
+      <c r="D31" s="5"/>
+      <c r="E31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="20"/>
+        <v>81</v>
+      </c>
+      <c r="D38" s="9"/>
       <c r="E38" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="7"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="9"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="8" t="s">
         <v>85</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
+      <c r="G39" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
       <c r="D41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="G41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="G42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6" t="s">
+      <c r="D44" s="5"/>
+      <c r="E44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="10"/>
-    </row>
     <row r="45" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="12" t="s">
+      <c r="B45" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="23" t="s">
+      <c r="C45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="D45" s="9"/>
+      <c r="E45" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0"/>
-      <c r="C46" s="0"/>
-      <c r="D46" s="0"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
       <c r="D47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="4" t="s">
+      <c r="G47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="G48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6" t="s">
+      <c r="D50" s="5"/>
+      <c r="E50" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G50" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>107</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F54" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>118</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F56" s="7"/>
+        <v>122</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59" s="12" t="s">
+    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="12" t="s">
+      <c r="C59" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="D59" s="9"/>
+      <c r="E59" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="F59" s="7" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="F60" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C61" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="C61" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G61" s="8"/>
-    </row>
-    <row r="62" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="25"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="26"/>
+        <v>152</v>
+      </c>
+      <c r="D64" s="9"/>
       <c r="E64" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D65" s="26"/>
       <c r="E65" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D66" s="26"/>
-      <c r="E66" s="10"/>
+      <c r="E66" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="F66" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D67" s="26"/>
       <c r="E67" s="10"/>
-      <c r="F67" s="7"/>
+      <c r="F67" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D68" s="26"/>
-      <c r="E68" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>166</v>
-      </c>
+      <c r="E68" s="10"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="D69" s="27"/>
+        <v>169</v>
+      </c>
+      <c r="D69" s="26"/>
       <c r="E69" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G69" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="s">
         <v>172</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="26"/>
+      <c r="D70" s="27"/>
       <c r="E70" s="8" t="s">
         <v>174</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G70" s="8"/>
-    </row>
-    <row r="71" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D71" s="26"/>
       <c r="E71" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D72" s="26"/>
       <c r="E72" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G72" s="8"/>
+    </row>
+    <row r="73" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D73" s="26"/>
+      <c r="E73" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="13"/>
+      <c r="E74" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>193</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B49:G49"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1" display="https://github.com/paramat/watershed"/>
+    <hyperlink ref="F46" r:id="rId1" display="https://github.com/paramat/watershed"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Mise à jour global des mods. Ajout des textures des joueurs de Steinheim dans le mod minetest-skin.
</commit_message>
<xml_diff>
--- a/steinheim 2.0 tableau des mods.xlsx
+++ b/steinheim 2.0 tableau des mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mods du gamemods" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="197">
   <si>
     <t>Aventure</t>
   </si>
@@ -320,6 +320,15 @@
     <t>SUPPRIMÉ : inhibe les mods farming_plus et mobs_redo</t>
   </si>
   <si>
+    <t>yappi</t>
+  </si>
+  <si>
+    <t>un autre mod de génération de map</t>
+  </si>
+  <si>
+    <t>https://github.com/SmallJoker/yappy.git</t>
+  </si>
+  <si>
     <t>Utilitaires</t>
   </si>
   <si>
@@ -596,7 +605,7 @@
     <t>https://github.com/jordan4ibanez/enchantment.git</t>
   </si>
   <si>
-    <t>ne fonctionne pas </t>
+    <t>ne fonctionne pas</t>
   </si>
 </sst>
 </file>
@@ -962,8 +971,8 @@
   </sheetPr>
   <dimension ref="B1:G74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E78" activeCellId="0" sqref="E78"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1580,9 +1589,16 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0"/>
-      <c r="C47" s="0"/>
+      <c r="B47" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="D47" s="0"/>
+      <c r="F47" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,7 +1609,7 @@
     </row>
     <row r="49" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="24"/>
@@ -1621,276 +1637,276 @@
     </row>
     <row r="51" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="8" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="11" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="12"/>
       <c r="F61" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G61" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="8" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D65" s="26"/>
       <c r="E65" s="8" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="8" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D67" s="26"/>
       <c r="E67" s="10"/>
       <c r="F67" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D68" s="26"/>
       <c r="E68" s="10"/>
@@ -1899,102 +1915,102 @@
     </row>
     <row r="69" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D70" s="27"/>
       <c r="E70" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D71" s="26"/>
       <c r="E71" s="8" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D72" s="26"/>
       <c r="E72" s="8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D73" s="26"/>
       <c r="E73" s="8" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="12" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>